<commit_message>
Done er and Booking layout in excel file
</commit_message>
<xml_diff>
--- a/TASKS.xlsx
+++ b/TASKS.xlsx
@@ -1432,8 +1432,8 @@
   </sheetPr>
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1479,7 +1479,7 @@
       <c r="A2" s="12"/>
       <c r="B2" s="36">
         <f ca="1">TODAY()</f>
-        <v>43753</v>
+        <v>43755</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="18"/>
@@ -1586,7 +1586,7 @@
       </c>
       <c r="D7" s="6">
         <f t="shared" ref="D7:D12" ca="1" si="0">TODAY()+4</f>
-        <v>43757</v>
+        <v>43759</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="D8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43757</v>
+        <v>43759</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
@@ -1626,13 +1626,15 @@
     </row>
     <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="35"/>
-      <c r="B9" s="9"/>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
       <c r="C9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="6">
         <f ca="1">TODAY()+3</f>
-        <v>43756</v>
+        <v>43758</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>5</v>
@@ -1654,7 +1656,7 @@
       </c>
       <c r="D10" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43757</v>
+        <v>43759</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>5</v>
@@ -1676,7 +1678,7 @@
       </c>
       <c r="D11" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43757</v>
+        <v>43759</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>5</v>
@@ -1698,7 +1700,7 @@
       </c>
       <c r="D12" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43757</v>
+        <v>43759</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>7</v>
@@ -1735,7 +1737,9 @@
       <c r="N13" s="2"/>
     </row>
     <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
+      <c r="B14" s="22">
+        <v>1</v>
+      </c>
       <c r="C14" s="23" t="s">
         <v>28</v>
       </c>
@@ -2068,21 +2072,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2294,14 +2298,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -2315,6 +2311,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
adding station manager layout
</commit_message>
<xml_diff>
--- a/TASKS.xlsx
+++ b/TASKS.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="23520" windowHeight="16596"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="23520" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="TASKS" sheetId="7" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="Grid" localSheetId="0">ToDoList[[#All],[Description]:[Assigned to]]</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">TASKS!$1:$6</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -137,14 +137,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="mm\.dd\.yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="166" formatCode="&quot;Done&quot;;&quot;&quot;;&quot;&quot;"/>
     <numFmt numFmtId="167" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.14996795556505021"/>
@@ -602,7 +602,6 @@
         <sz val="14"/>
         <color theme="0"/>
         <name val="Rockwell"/>
-        <family val="1"/>
         <scheme val="major"/>
       </font>
     </dxf>
@@ -633,7 +632,6 @@
         <sz val="11"/>
         <color theme="1" tint="0.14996795556505021"/>
         <name val="Rockwell"/>
-        <family val="1"/>
         <scheme val="major"/>
       </font>
     </dxf>
@@ -806,7 +804,7 @@
         <xdr:cNvPr id="4" name="Data Entry Tip" descr="Enter a number greater than 1 in Done column when  task is complete">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -883,7 +881,7 @@
         <xdr:cNvPr id="16" name="Data Entry Tip" descr="Enter a number greater than 1 in Done column when  task is complete">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1954A24D-DF3A-439E-AB30-634556E8A9EB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1954A24D-DF3A-439E-AB30-634556E8A9EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1052,7 +1050,7 @@
         <xdr:cNvPr id="17" name="Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF377864-4FEB-4775-90CF-2A6C6DFF8FD2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF377864-4FEB-4775-90CF-2A6C6DFF8FD2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1067,7 +1065,7 @@
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{837473B0-CC2E-450A-ABE3-18F120FF3D39}">
-              <a1611:picAttrSrcUrl xmlns:a1611="http://schemas.microsoft.com/office/drawing/2016/11/main" r:id="rId2"/>
+              <a1611:picAttrSrcUrl xmlns:a1611="http://schemas.microsoft.com/office/drawing/2016/11/main" xmlns="" r:id="rId2"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1110,7 +1108,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2770D6CE-90D9-4DCF-B559-472B60DCF791}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2770D6CE-90D9-4DCF-B559-472B60DCF791}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1433,26 +1431,26 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.81640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="30.6328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.90625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="7.7265625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20.26953125" style="2" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.26953125" style="4" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="1.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="7.77734375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" style="2" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.21875" style="4" hidden="1" customWidth="1"/>
     <col min="10" max="14" width="0" style="4" hidden="1" customWidth="1"/>
     <col min="15" max="17" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.7265625" style="2" hidden="1"/>
+    <col min="18" max="16384" width="10.77734375" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="66" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1475,7 +1473,7 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" ht="21.75" customHeight="1">
       <c r="A2" s="12"/>
       <c r="B2" s="36">
         <f ca="1">TODAY()</f>
@@ -1494,7 +1492,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="23.25" customHeight="1">
       <c r="A3" s="13"/>
       <c r="B3" s="33" t="s">
         <v>14</v>
@@ -1515,7 +1513,7 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="23.25" customHeight="1">
       <c r="A4" s="13"/>
       <c r="B4" s="34" t="s">
         <v>15</v>
@@ -1536,7 +1534,7 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
     </row>
-    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" ht="12.75" customHeight="1">
       <c r="B5" s="7"/>
       <c r="C5" s="14"/>
       <c r="D5" s="11"/>
@@ -1550,7 +1548,7 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:17" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="16" customFormat="1" ht="30" customHeight="1">
       <c r="A6" s="15"/>
       <c r="B6" s="19" t="s">
         <v>2</v>
@@ -1574,12 +1572,12 @@
       <c r="N6" s="15"/>
       <c r="O6" s="15"/>
     </row>
-    <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="30" customHeight="1">
       <c r="A7" s="35" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>24</v>
@@ -1601,7 +1599,7 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="30" customHeight="1">
       <c r="A8" s="35"/>
       <c r="B8" s="9"/>
       <c r="C8" s="8" t="s">
@@ -1624,7 +1622,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="30" customHeight="1">
       <c r="A9" s="35"/>
       <c r="B9" s="9">
         <v>1</v>
@@ -1649,7 +1647,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="30" customHeight="1">
       <c r="B10" s="9"/>
       <c r="C10" s="8" t="s">
         <v>27</v>
@@ -1671,7 +1669,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:17" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="30" hidden="1" customHeight="1">
       <c r="B11" s="9"/>
       <c r="C11" s="8" t="s">
         <v>8</v>
@@ -1693,7 +1691,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="30" hidden="1" customHeight="1">
       <c r="B12" s="9"/>
       <c r="C12" s="8" t="s">
         <v>10</v>
@@ -1715,7 +1713,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="30" customHeight="1">
       <c r="B13" s="22"/>
       <c r="C13" s="23" t="s">
         <v>28</v>
@@ -1736,7 +1734,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="30" customHeight="1">
       <c r="B14" s="22">
         <v>1</v>
       </c>
@@ -1759,7 +1757,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="30" customHeight="1">
       <c r="B15" s="22"/>
       <c r="C15" s="23" t="s">
         <v>28</v>
@@ -1780,7 +1778,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="30" customHeight="1">
       <c r="B16" s="22"/>
       <c r="C16" s="23" t="s">
         <v>28</v>
@@ -1801,7 +1799,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" ht="30" customHeight="1">
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1814,7 +1812,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" ht="30" customHeight="1">
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1827,7 +1825,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" ht="30" customHeight="1">
       <c r="B19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1840,7 +1838,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" ht="30" customHeight="1">
       <c r="B20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1853,7 +1851,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" ht="30" customHeight="1">
       <c r="B21" s="2"/>
       <c r="C21" s="4"/>
       <c r="H21" s="4"/>
@@ -1864,7 +1862,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" ht="30" customHeight="1">
       <c r="B22" s="2"/>
       <c r="C22" s="4"/>
       <c r="H22" s="4"/>
@@ -1969,18 +1967,18 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.81640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.77734375" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" style="2" customWidth="1"/>
-    <col min="4" max="6" width="8.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="7.1796875" style="2" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" style="2" customWidth="1"/>
+    <col min="4" max="6" width="8.77734375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" style="2" hidden="1" customWidth="1"/>
     <col min="8" max="15" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.7265625" style="2" hidden="1"/>
+    <col min="16" max="16384" width="10.77734375" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" ht="66" customHeight="1">
       <c r="B1" s="39" t="s">
         <v>11</v>
       </c>
@@ -1996,7 +1994,7 @@
       <c r="J1" s="17"/>
       <c r="K1" s="17"/>
     </row>
-    <row r="2" spans="2:11" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" ht="83.25" customHeight="1">
       <c r="B2" s="38" t="s">
         <v>16</v>
       </c>
@@ -2010,7 +2008,7 @@
       <c r="J2" s="17"/>
       <c r="K2" s="17"/>
     </row>
-    <row r="3" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="30" customHeight="1">
       <c r="B3" s="21" t="s">
         <v>12</v>
       </c>
@@ -2018,31 +2016,31 @@
       <c r="E3" s="37"/>
       <c r="F3" s="37"/>
     </row>
-    <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="30" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="30" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="30" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="30" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="30" customHeight="1">
       <c r="B8" s="5"/>
       <c r="E8" s="20"/>
     </row>
-    <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="30" customHeight="1">
       <c r="B9" s="5"/>
     </row>
   </sheetData>
@@ -2072,21 +2070,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2298,6 +2296,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -2311,14 +2317,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add Abobakr's ER Diagram
</commit_message>
<xml_diff>
--- a/TASKS.xlsx
+++ b/TASKS.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADF4E3A-3913-4E2E-B275-486253A5E0CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="23520" windowHeight="16440"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TASKS" sheetId="7" r:id="rId1"/>
@@ -25,12 +26,19 @@
     <definedName name="Grid" localSheetId="0">ToDoList[[#All],[Description]:[Assigned to]]</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">TASKS!$1:$6</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t xml:space="preserve">                            </t>
   </si>
@@ -137,7 +145,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="mm\.dd\.yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -572,7 +580,7 @@
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
-    <cellStyle name="Date" xfId="11"/>
+    <cellStyle name="Date" xfId="11" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Explanatory Text" xfId="7" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
@@ -580,7 +588,7 @@
     <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Phone" xfId="10"/>
+    <cellStyle name="Phone" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="8" builtinId="25" customBuiltin="1"/>
   </cellStyles>
@@ -612,7 +620,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="168" formatCode="m/d/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -755,13 +763,13 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="To Do List" defaultPivotStyle="PivotStyleLight18">
-    <tableStyle name="Address Book" pivot="0" count="4">
+    <tableStyle name="Address Book" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="18"/>
       <tableStyleElement type="headerRow" dxfId="17"/>
       <tableStyleElement type="firstRowStripe" dxfId="16"/>
       <tableStyleElement type="secondRowStripe" dxfId="15"/>
     </tableStyle>
-    <tableStyle name="To Do List" pivot="0" count="2">
+    <tableStyle name="To Do List" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="wholeTable" dxfId="14"/>
       <tableStyleElement type="headerRow" dxfId="13"/>
     </tableStyle>
@@ -804,7 +812,7 @@
         <xdr:cNvPr id="4" name="Data Entry Tip" descr="Enter a number greater than 1 in Done column when  task is complete">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -881,7 +889,7 @@
         <xdr:cNvPr id="16" name="Data Entry Tip" descr="Enter a number greater than 1 in Done column when  task is complete">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1954A24D-DF3A-439E-AB30-634556E8A9EB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1954A24D-DF3A-439E-AB30-634556E8A9EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1050,7 +1058,7 @@
         <xdr:cNvPr id="17" name="Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF377864-4FEB-4775-90CF-2A6C6DFF8FD2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF377864-4FEB-4775-90CF-2A6C6DFF8FD2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1065,7 +1073,7 @@
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
             <a:ext uri="{837473B0-CC2E-450A-ABE3-18F120FF3D39}">
-              <a1611:picAttrSrcUrl xmlns:a1611="http://schemas.microsoft.com/office/drawing/2016/11/main" xmlns="" r:id="rId2"/>
+              <a1611:picAttrSrcUrl xmlns:a1611="http://schemas.microsoft.com/office/drawing/2016/11/main" r:id="rId2"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1108,7 +1116,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2770D6CE-90D9-4DCF-B559-472B60DCF791}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2770D6CE-90D9-4DCF-B559-472B60DCF791}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1154,8 +1162,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ToDoList" displayName="ToDoList" ref="B6:F16" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="B6:F16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="ToDoList" displayName="ToDoList" ref="B6:F16" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="B6:F16" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="4">
       <filters>
         <filter val="AboZ"/>
@@ -1166,13 +1174,13 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name="Done" dataDxfId="6"/>
-    <tableColumn id="2" name="Description" dataDxfId="5"/>
-    <tableColumn id="3" name="Due Date" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Done" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Due Date" dataDxfId="4">
       <calculatedColumnFormula>TODAY()+4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Priority" dataDxfId="3"/>
-    <tableColumn id="5" name="Assigned to" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Priority" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Assigned to" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1184,9 +1192,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="ColorKeys" displayName="ColorKeys" ref="B3:B9" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="ColorKeys" displayName="ColorKeys" ref="B3:B9" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
   <tableColumns count="1">
-    <tableColumn id="1" name="Assigned To"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Assigned To"/>
   </tableColumns>
   <tableStyleInfo name="Address Book" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1423,7 +1431,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <tabColor theme="7" tint="0.59999389629810485"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
@@ -1431,23 +1439,23 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="7.77734375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="20.21875" style="2" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.21875" style="4" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="1.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="30.6328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.90625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="7.81640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" style="2" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1796875" style="4" hidden="1" customWidth="1"/>
     <col min="10" max="14" width="0" style="4" hidden="1" customWidth="1"/>
     <col min="15" max="17" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.77734375" style="2" hidden="1"/>
+    <col min="18" max="16384" width="10.81640625" style="2" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="66" customHeight="1">
@@ -1477,7 +1485,7 @@
       <c r="A2" s="12"/>
       <c r="B2" s="36">
         <f ca="1">TODAY()</f>
-        <v>43755</v>
+        <v>43756</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="18"/>
@@ -1584,7 +1592,7 @@
       </c>
       <c r="D7" s="6">
         <f t="shared" ref="D7:D12" ca="1" si="0">TODAY()+4</f>
-        <v>43759</v>
+        <v>43760</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
@@ -1601,13 +1609,15 @@
     </row>
     <row r="8" spans="1:17" ht="30" customHeight="1">
       <c r="A8" s="35"/>
-      <c r="B8" s="9"/>
+      <c r="B8" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="C8" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43759</v>
+        <v>43760</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
@@ -1632,7 +1642,7 @@
       </c>
       <c r="D9" s="6">
         <f ca="1">TODAY()+3</f>
-        <v>43758</v>
+        <v>43759</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>5</v>
@@ -1654,7 +1664,7 @@
       </c>
       <c r="D10" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43759</v>
+        <v>43760</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>5</v>
@@ -1676,7 +1686,7 @@
       </c>
       <c r="D11" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43759</v>
+        <v>43760</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>5</v>
@@ -1698,7 +1708,7 @@
       </c>
       <c r="D12" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>43759</v>
+        <v>43760</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>7</v>
@@ -1714,7 +1724,9 @@
       <c r="N12" s="2"/>
     </row>
     <row r="13" spans="1:17" ht="30" customHeight="1">
-      <c r="B13" s="22"/>
+      <c r="B13" s="22" t="s">
+        <v>2</v>
+      </c>
       <c r="C13" s="23" t="s">
         <v>28</v>
       </c>
@@ -1898,30 +1910,30 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="17">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select Priority from the list. Select CANCEL, press ALT+DOWN ARROW for options, then DOWN ARROW and ENTER to make selection" sqref="E7:E16">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select Priority from the list. Select CANCEL, press ALT+DOWN ARROW for options, then DOWN ARROW and ENTER to make selection" sqref="E7:E16" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select Assigned to names from the list. Select CANCEL, press ALT+DOWN ARROW for options, then DOWN ARROW and ENTER to make selection" sqref="F7:F16">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select Assigned to names from the list. Select CANCEL, press ALT+DOWN ARROW for options, then DOWN ARROW and ENTER to make selection" sqref="F7:F16" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>Assignedto</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create To Do List in this workbook. Enter details in To Do List table in this worksheet. Select cell F1 to navigate to Setup worksheet. Due &amp; Overdue days are automatically updated" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to Assignment Setup worksheet" sqref="F1:G5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Date is automatically updated in this cell and Due Today and Overdue days in cells below" sqref="B2:C2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Due Today is automatically updated in cell at right" sqref="B3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Due Today is automatically updated in this cell" sqref="C3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Description in this column under this heading" sqref="C6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Due Date in this column under this heading" sqref="D6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Priority in this column under this heading. Press ALT+DOWN ARROW for options, then DOWN ARROW and ENTER to make selection" sqref="E6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Assigned to names in this column under this heading. Press ALT+DOWN ARROW for options, then DOWN ARROW and ENTER to make selection" sqref="F6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter value greater than 1 in this column under this heading to mark task as Done. Strikethrough formatting will automatically be applied" sqref="B6"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Date is automatically updated in cell below, and Due Today and Overdue days in cell C3 and C4. Tip is in cell at right" sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this C1. Date is automatically updated in cell B2, and Due Today and Overdue days in cell C3 and C4. Next tip is in cell below." sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Overdue days are automatically updated in cell at right" sqref="B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Overdue days are automatically updated in this cell. Enter details in table below. Table tip is in cell A6" sqref="C4"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B5:C5"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create To Do List in this workbook. Enter details in To Do List table in this worksheet. Select cell F1 to navigate to Setup worksheet. Due &amp; Overdue days are automatically updated" sqref="A1" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to Assignment Setup worksheet" sqref="F1:G5" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Date is automatically updated in this cell and Due Today and Overdue days in cells below" sqref="B2:C2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Due Today is automatically updated in cell at right" sqref="B3" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Due Today is automatically updated in this cell" sqref="C3" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Description in this column under this heading" sqref="C6" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Due Date in this column under this heading" sqref="D6" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Priority in this column under this heading. Press ALT+DOWN ARROW for options, then DOWN ARROW and ENTER to make selection" sqref="E6" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Assigned to names in this column under this heading. Press ALT+DOWN ARROW for options, then DOWN ARROW and ENTER to make selection" sqref="F6" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter value greater than 1 in this column under this heading to mark task as Done. Strikethrough formatting will automatically be applied" sqref="B6" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Date is automatically updated in cell below, and Due Today and Overdue days in cell C3 and C4. Tip is in cell at right" sqref="C1" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this C1. Date is automatically updated in cell B2, and Due Today and Overdue days in cell C3 and C4. Next tip is in cell below." sqref="B1" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Overdue days are automatically updated in cell at right" sqref="B4" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Overdue days are automatically updated in this cell. Enter details in table below. Table tip is in cell A6" sqref="C4" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B5:C5" xr:uid="{00000000-0002-0000-0000-000010000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F1" location="'Assignment Setup'!A1" tooltip="Click to navigate to TAssignment Setup" display="Setup &gt;"/>
+    <hyperlink ref="F1" location="'Assignment Setup'!A1" tooltip="Click to navigate to TAssignment Setup" display="Setup &gt;" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="58" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -1958,7 +1970,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="TaskSetup">
     <tabColor theme="6" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1969,13 +1981,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" style="2" customWidth="1"/>
-    <col min="4" max="6" width="8.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="7.21875" style="2" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" style="2" customWidth="1"/>
+    <col min="4" max="6" width="8.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="7.1796875" style="2" hidden="1" customWidth="1"/>
     <col min="8" max="15" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.77734375" style="2" hidden="1"/>
+    <col min="16" max="16384" width="10.81640625" style="2" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="66" customHeight="1">
@@ -2051,14 +2063,14 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create an Assignment Setup in this worksheet. Insert or modify entries in Color Keys table starting in cell B4. Select cell G1 to navigate to To Do List. Tip is in cell B2" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insert or modify Assigned To names in this column under this heading" sqref="B3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell, tip in cell below, and navigation link to To Do List worksheet in cell at right" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to To Do List worksheet" sqref="E1 G1:K2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create an Assignment Setup in this worksheet. Insert or modify entries in Color Keys table starting in cell B4. Select cell G1 to navigate to To Do List. Tip is in cell B2" sqref="A1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insert or modify Assigned To names in this column under this heading" sqref="B3" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell, tip in cell below, and navigation link to To Do List worksheet in cell at right" sqref="B1" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Navigation link to To Do List worksheet" sqref="E1 G1:K2" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G1:K2" location="'To Do List'!A1" tooltip="Select to navigate to To Do List worksheet" display="&lt; To Do List"/>
-    <hyperlink ref="E1:F1" location="'To Do List'!A1" tooltip="Click to navigate to To Do List worksheet" display="&lt; To Do List"/>
+    <hyperlink ref="G1:K2" location="'To Do List'!A1" tooltip="Select to navigate to To Do List worksheet" display="&lt; To Do List" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E1:F1" location="'To Do List'!A1" tooltip="Click to navigate to To Do List worksheet" display="&lt; To Do List" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2079,15 +2091,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3b47856d4cf355c0dacb39e1084d14f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a845a615265fdb1f7b12cc65ac20ecbd" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2295,6 +2298,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
   <ds:schemaRefs>
@@ -2304,24 +2316,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6dc4bcd6-49db-4c07-9060-8acfc67cef9f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fb0879af-3eba-417a-a55a-ffe6dcd6ca77"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7118F064-9046-4DCB-A010-2D274D0FB549}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2339,4 +2333,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6dc4bcd6-49db-4c07-9060-8acfc67cef9f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb0879af-3eba-417a-a55a-ffe6dcd6ca77"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Repair yard and Routes procedure added update station procedure
</commit_message>
<xml_diff>
--- a/TASKS.xlsx
+++ b/TASKS.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B94EF1-9B10-43B4-9E83-A88D3592AEDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B92A11-A674-48E1-918D-83C2DF6FF1DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <definedName name="Grid" localSheetId="0">ToDoList[[#All],[Description]:[Assigned to]]</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">TASKS!$1:$6</definedName>
   </definedNames>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -141,7 +141,7 @@
     <numFmt numFmtId="166" formatCode="&quot;Done&quot;;&quot;&quot;;&quot;&quot;"/>
     <numFmt numFmtId="167" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.14996795556505021"/>
@@ -612,7 +612,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="168" formatCode="m/d/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1431,10 +1431,10 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="1.81640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.453125" style="4" customWidth="1"/>
@@ -1450,7 +1450,7 @@
     <col min="18" max="16384" width="10.81640625" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="66" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1473,7 +1473,7 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" ht="21.75" customHeight="1">
       <c r="A2" s="12"/>
       <c r="B2" s="37">
         <f ca="1">TODAY()</f>
@@ -1492,7 +1492,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="23.25" customHeight="1">
       <c r="A3" s="13"/>
       <c r="B3" s="33" t="s">
         <v>9</v>
@@ -1513,7 +1513,7 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="23.25" customHeight="1">
       <c r="A4" s="13"/>
       <c r="B4" s="34" t="s">
         <v>10</v>
@@ -1534,7 +1534,7 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
     </row>
-    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" ht="12.75" customHeight="1">
       <c r="B5" s="7"/>
       <c r="C5" s="14"/>
       <c r="D5" s="11"/>
@@ -1548,7 +1548,7 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:17" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="16" customFormat="1" ht="30" customHeight="1">
       <c r="A6" s="15"/>
       <c r="B6" s="19" t="s">
         <v>2</v>
@@ -1572,7 +1572,7 @@
       <c r="N6" s="15"/>
       <c r="O6" s="15"/>
     </row>
-    <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="30" customHeight="1">
       <c r="A7" s="36" t="s">
         <v>12</v>
       </c>
@@ -1596,10 +1596,10 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="30" customHeight="1">
       <c r="A8" s="36"/>
       <c r="B8" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>24</v>
@@ -1618,7 +1618,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="30" customHeight="1">
       <c r="A9" s="36"/>
       <c r="B9" s="9">
         <v>1</v>
@@ -1640,7 +1640,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="30" customHeight="1">
       <c r="B10" s="9"/>
       <c r="C10" s="35" t="s">
         <v>25</v>
@@ -1657,7 +1657,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:17" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="30" hidden="1" customHeight="1">
       <c r="B11" s="9"/>
       <c r="C11" s="8"/>
       <c r="D11" s="6"/>
@@ -1670,7 +1670,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="30" hidden="1" customHeight="1">
       <c r="B12" s="9"/>
       <c r="C12" s="8"/>
       <c r="D12" s="6"/>
@@ -1683,7 +1683,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="30" customHeight="1">
       <c r="B13" s="22">
         <v>0</v>
       </c>
@@ -1702,7 +1702,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="30" customHeight="1">
       <c r="B14" s="22">
         <v>0</v>
       </c>
@@ -1721,7 +1721,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="30" customHeight="1">
       <c r="B15" s="22"/>
       <c r="C15" s="23"/>
       <c r="D15" s="24"/>
@@ -1734,7 +1734,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="30" customHeight="1">
       <c r="B16" s="22"/>
       <c r="C16" s="23"/>
       <c r="D16" s="24"/>
@@ -1747,7 +1747,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" ht="30" customHeight="1">
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1760,7 +1760,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" ht="30" customHeight="1">
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1773,7 +1773,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" ht="30" customHeight="1">
       <c r="B19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1786,7 +1786,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" ht="30" customHeight="1">
       <c r="B20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1799,7 +1799,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" ht="30" customHeight="1">
       <c r="B21" s="2"/>
       <c r="C21" s="4"/>
       <c r="H21" s="4"/>
@@ -1810,7 +1810,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" ht="30" customHeight="1">
       <c r="B22" s="2"/>
       <c r="C22" s="4"/>
       <c r="H22" s="4"/>
@@ -1917,7 +1917,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.81640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
@@ -1928,7 +1928,7 @@
     <col min="16" max="16384" width="10.81640625" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" ht="66" customHeight="1">
       <c r="B1" s="40" t="s">
         <v>6</v>
       </c>
@@ -1944,7 +1944,7 @@
       <c r="J1" s="17"/>
       <c r="K1" s="17"/>
     </row>
-    <row r="2" spans="2:11" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" ht="83.25" customHeight="1">
       <c r="B2" s="39" t="s">
         <v>11</v>
       </c>
@@ -1958,7 +1958,7 @@
       <c r="J2" s="17"/>
       <c r="K2" s="17"/>
     </row>
-    <row r="3" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="30" customHeight="1">
       <c r="B3" s="21" t="s">
         <v>7</v>
       </c>
@@ -1966,31 +1966,31 @@
       <c r="E3" s="38"/>
       <c r="F3" s="38"/>
     </row>
-    <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="30" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="30" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="30" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="30" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="30" customHeight="1">
       <c r="B8" s="5"/>
       <c r="E8" s="20"/>
     </row>
-    <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="30" customHeight="1">
       <c r="B9" s="5"/>
     </row>
   </sheetData>
@@ -2029,6 +2029,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3b47856d4cf355c0dacb39e1084d14f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a845a615265fdb1f7b12cc65ac20ecbd" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2236,15 +2245,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
   <ds:schemaRefs>
@@ -2254,6 +2254,24 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6dc4bcd6-49db-4c07-9060-8acfc67cef9f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb0879af-3eba-417a-a55a-ffe6dcd6ca77"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7118F064-9046-4DCB-A010-2D274D0FB549}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2271,22 +2289,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6dc4bcd6-49db-4c07-9060-8acfc67cef9f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fb0879af-3eba-417a-a55a-ffe6dcd6ca77"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>